<commit_message>
v20180806 #20 21 22 23
</commit_message>
<xml_diff>
--- a/doc/env.xlsx
+++ b/doc/env.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="161">
   <si>
     <t>【mysql】</t>
     <phoneticPr fontId="1"/>
@@ -1013,10 +1013,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>版本：v20180730</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>手动变更</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1049,6 +1045,22 @@
   </si>
   <si>
     <t>ADD unit_tbl::c_type INT 未设定类别(1) 货币单位类别(2)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADD order_tbl::c_price_unit_id INT 单价单位ID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADD pn_tbl::c_price FLOAT 单价</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADD pn_tbl::c_price_unit_id INT 单价单位ID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>版本：v20180806</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1631,11 +1643,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD49"/>
+  <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1644,7 +1654,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
@@ -1717,22 +1727,22 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="E5" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="E6" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
@@ -1742,604 +1752,622 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="B8" s="5"/>
+      <c r="E8" s="4" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>152</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="E9" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
       <c r="B10" s="5"/>
+      <c r="E10" s="4" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>154</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="8"/>
-    </row>
-    <row r="13" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="8"/>
+    </row>
+    <row r="16" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-    </row>
-    <row r="14" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+    </row>
+    <row r="17" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="E17" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="E18" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
-      <c r="E19" s="4" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="E20" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B21" s="5"/>
+      <c r="E21" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="E22" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B23" s="5"/>
+      <c r="E23" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8" t="s">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="8"/>
-      <c r="AB23" s="8"/>
-      <c r="AC23" s="8"/>
-      <c r="AD23" s="8"/>
-    </row>
-    <row r="24" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8"/>
+    </row>
+    <row r="27" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-    </row>
-    <row r="25" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="11"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="11"/>
+    </row>
+    <row r="28" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="11"/>
-      <c r="AB25" s="11"/>
-      <c r="AC25" s="11"/>
-      <c r="AD25" s="11"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="s">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B32" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8" t="s">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="8"/>
-      <c r="AB31" s="8"/>
-      <c r="AC31" s="8"/>
-      <c r="AD31" s="8"/>
-    </row>
-    <row r="32" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+      <c r="AA34" s="8"/>
+      <c r="AB34" s="8"/>
+      <c r="AC34" s="8"/>
+      <c r="AD34" s="8"/>
+    </row>
+    <row r="35" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="11" t="s">
+      <c r="B35" s="10"/>
+      <c r="C35" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="11"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-    </row>
-    <row r="33" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+    </row>
+    <row r="36" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B35" s="5" t="s">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B38" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B36" s="5" t="s">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B39" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B37" s="5" t="s">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8" t="s">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-      <c r="AA39" s="8"/>
-      <c r="AB39" s="8"/>
-      <c r="AC39" s="8"/>
-      <c r="AD39" s="8"/>
-    </row>
-    <row r="40" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
+      <c r="Z42" s="8"/>
+      <c r="AA42" s="8"/>
+      <c r="AB42" s="8"/>
+      <c r="AC42" s="8"/>
+      <c r="AD42" s="8"/>
+    </row>
+    <row r="43" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="11" t="s">
+      <c r="B43" s="10"/>
+      <c r="C43" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
-      <c r="V40" s="11"/>
-      <c r="W40" s="11"/>
-      <c r="X40" s="11"/>
-      <c r="Y40" s="11"/>
-      <c r="Z40" s="11"/>
-      <c r="AA40" s="11"/>
-      <c r="AB40" s="11"/>
-      <c r="AC40" s="11"/>
-      <c r="AD40" s="11"/>
-    </row>
-    <row r="41" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="11"/>
+      <c r="AB43" s="11"/>
+      <c r="AC43" s="11"/>
+      <c r="AD43" s="11"/>
+    </row>
+    <row r="44" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="11"/>
-      <c r="V41" s="11"/>
-      <c r="W41" s="11"/>
-      <c r="X41" s="11"/>
-      <c r="Y41" s="11"/>
-      <c r="Z41" s="11"/>
-      <c r="AA41" s="11"/>
-      <c r="AB41" s="11"/>
-      <c r="AC41" s="11"/>
-      <c r="AD41" s="11"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
+      <c r="AA44" s="11"/>
+      <c r="AB44" s="11"/>
+      <c r="AC44" s="11"/>
+      <c r="AD44" s="11"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B43" s="5" t="s">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B44" s="5" t="s">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B47" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B46" s="4" t="s">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B49" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B48" s="4" t="s">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
-      <c r="B49" s="9" t="s">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="8"/>
-      <c r="W49" s="8"/>
-      <c r="X49" s="8"/>
-      <c r="Y49" s="8"/>
-      <c r="Z49" s="8"/>
-      <c r="AA49" s="8"/>
-      <c r="AB49" s="8"/>
-      <c r="AC49" s="8"/>
-      <c r="AD49" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="8"/>
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="8"/>
+      <c r="AD52" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
v20180818 #47 #48 #49 #51 #56 #57 #60 #61
</commit_message>
<xml_diff>
--- a/doc/env.xlsx
+++ b/doc/env.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,12 +13,12 @@
     <sheet name="mysql" sheetId="1" r:id="rId4"/>
     <sheet name="my.ini" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="163">
   <si>
     <t>【mysql】</t>
     <phoneticPr fontId="1"/>
@@ -79,7 +79,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -90,7 +90,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -108,7 +108,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -119,7 +119,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -130,7 +130,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -154,7 +154,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -165,7 +165,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -176,7 +176,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -197,7 +197,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -208,7 +208,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -344,7 +344,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -355,7 +355,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -365,7 +365,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -376,7 +376,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -387,7 +387,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -447,7 +447,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -458,7 +458,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -476,7 +476,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -487,7 +487,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -520,7 +520,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -531,7 +531,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -552,7 +552,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -563,7 +563,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -653,7 +653,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -664,7 +664,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -694,7 +694,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -705,7 +705,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -715,7 +715,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -731,7 +731,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -742,7 +742,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -752,7 +752,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -763,7 +763,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -803,7 +803,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -820,7 +820,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -837,7 +837,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -848,7 +848,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -859,7 +859,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -876,7 +876,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -887,7 +887,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -897,7 +897,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -908,7 +908,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1061,6 +1061,14 @@
   </si>
   <si>
     <t>版本：v20180806</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>版本：v20180818</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ADD entry_bom_tbl::c_supplier_id INT NOT NULL DEFAULT(0) 供应商ID</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1068,17 +1076,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1086,7 +1094,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1101,7 +1109,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1114,7 +1122,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1141,7 +1149,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1149,7 +1157,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1238,7 +1246,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1357,7 +1365,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1399,7 +1407,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1434,7 +1442,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1643,18 +1651,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD52"/>
+  <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="2.75" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="12" customFormat="1">
       <c r="A1" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
@@ -1686,7 +1696,7 @@
       <c r="AC1" s="11"/>
       <c r="AD1" s="11"/>
     </row>
-    <row r="2" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" s="12" customFormat="1">
       <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
@@ -1720,354 +1730,354 @@
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30">
       <c r="A3" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30">
       <c r="B4" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:30">
+      <c r="A6" s="13"/>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+    </row>
+    <row r="9" spans="1:30" s="12" customFormat="1">
+      <c r="A9" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+    </row>
+    <row r="10" spans="1:30" s="12" customFormat="1">
+      <c r="A10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="B12" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="E5" s="4" t="s">
+    <row r="13" spans="1:30">
+      <c r="B13" s="5"/>
+      <c r="E13" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="E6" s="4" t="s">
+    <row r="14" spans="1:30">
+      <c r="B14" s="5"/>
+      <c r="E14" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B7" s="5"/>
-      <c r="E7" s="4" t="s">
+    <row r="15" spans="1:30">
+      <c r="B15" s="5"/>
+      <c r="E15" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B8" s="5"/>
-      <c r="E8" s="4" t="s">
+    <row r="16" spans="1:30">
+      <c r="B16" s="5"/>
+      <c r="E16" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="E9" s="4" t="s">
+    <row r="17" spans="1:30">
+      <c r="B17" s="5"/>
+      <c r="E17" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B10" s="5"/>
-      <c r="E10" s="4" t="s">
+    <row r="18" spans="1:30">
+      <c r="B18" s="5"/>
+      <c r="E18" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="19" spans="1:30">
+      <c r="A19" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="B20" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="21" spans="1:30">
+      <c r="A21" s="13"/>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8" t="s">
+    <row r="23" spans="1:30">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-    </row>
-    <row r="16" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8"/>
+    </row>
+    <row r="24" spans="1:30" s="12" customFormat="1">
+      <c r="A24" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-    </row>
-    <row r="17" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+    </row>
+    <row r="25" spans="1:30" s="12" customFormat="1">
+      <c r="A25" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
+    <row r="27" spans="1:30">
+      <c r="B27" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
-      <c r="E20" s="4" t="s">
+    <row r="28" spans="1:30">
+      <c r="B28" s="5"/>
+      <c r="E28" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="E21" s="4" t="s">
+    <row r="29" spans="1:30">
+      <c r="B29" s="5"/>
+      <c r="E29" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
-      <c r="E22" s="4" t="s">
+    <row r="30" spans="1:30">
+      <c r="B30" s="5"/>
+      <c r="E30" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
-      <c r="E23" s="4" t="s">
+    <row r="31" spans="1:30">
+      <c r="B31" s="5"/>
+      <c r="E31" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-      <c r="W26" s="8"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8"/>
-      <c r="AB26" s="8"/>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
-    </row>
-    <row r="27" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="11"/>
-    </row>
-    <row r="28" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
-      <c r="AD28" s="11"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B30" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30">
+      <c r="A32" s="13"/>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:30">
       <c r="A33" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30">
       <c r="A34" s="8"/>
       <c r="B34" s="8" t="s">
         <v>136</v>
@@ -2101,14 +2111,12 @@
       <c r="AC34" s="8"/>
       <c r="AD34" s="8"/>
     </row>
-    <row r="35" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" s="12" customFormat="1">
       <c r="A35" s="10" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="B35" s="10"/>
-      <c r="C35" s="11" t="s">
-        <v>131</v>
-      </c>
+      <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -2137,7 +2145,7 @@
       <c r="AC35" s="11"/>
       <c r="AD35" s="11"/>
     </row>
-    <row r="36" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" s="12" customFormat="1">
       <c r="A36" s="11" t="s">
         <v>51</v>
       </c>
@@ -2171,32 +2179,32 @@
       <c r="AC36" s="11"/>
       <c r="AD36" s="11"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30">
       <c r="A37" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30">
       <c r="B38" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30">
       <c r="B39" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30">
       <c r="B40" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30">
       <c r="A41" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
         <v>136</v>
@@ -2230,13 +2238,13 @@
       <c r="AC42" s="8"/>
       <c r="AD42" s="8"/>
     </row>
-    <row r="43" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" s="12" customFormat="1">
       <c r="A43" s="10" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="11" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
@@ -2266,7 +2274,7 @@
       <c r="AC43" s="11"/>
       <c r="AD43" s="11"/>
     </row>
-    <row r="44" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" s="12" customFormat="1">
       <c r="A44" s="11" t="s">
         <v>51</v>
       </c>
@@ -2300,74 +2308,203 @@
       <c r="AC44" s="11"/>
       <c r="AD44" s="11"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30">
       <c r="A45" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30">
+      <c r="B46" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30">
+      <c r="B47" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30">
+      <c r="B48" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30">
+      <c r="A49" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="8"/>
+      <c r="X50" s="8"/>
+      <c r="Y50" s="8"/>
+      <c r="Z50" s="8"/>
+      <c r="AA50" s="8"/>
+      <c r="AB50" s="8"/>
+      <c r="AC50" s="8"/>
+      <c r="AD50" s="8"/>
+    </row>
+    <row r="51" spans="1:30" s="12" customFormat="1">
+      <c r="A51" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+      <c r="U51" s="11"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="11"/>
+      <c r="X51" s="11"/>
+      <c r="Y51" s="11"/>
+      <c r="Z51" s="11"/>
+      <c r="AA51" s="11"/>
+      <c r="AB51" s="11"/>
+      <c r="AC51" s="11"/>
+      <c r="AD51" s="11"/>
+    </row>
+    <row r="52" spans="1:30" s="12" customFormat="1">
+      <c r="A52" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
+      <c r="T52" s="11"/>
+      <c r="U52" s="11"/>
+      <c r="V52" s="11"/>
+      <c r="W52" s="11"/>
+      <c r="X52" s="11"/>
+      <c r="Y52" s="11"/>
+      <c r="Z52" s="11"/>
+      <c r="AA52" s="11"/>
+      <c r="AB52" s="11"/>
+      <c r="AC52" s="11"/>
+      <c r="AD52" s="11"/>
+    </row>
+    <row r="53" spans="1:30">
+      <c r="A53" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B46" s="5" t="s">
+    <row r="54" spans="1:30">
+      <c r="B54" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B47" s="5" t="s">
+    <row r="55" spans="1:30">
+      <c r="B55" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+    <row r="56" spans="1:30">
+      <c r="A56" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
+    <row r="57" spans="1:30">
+      <c r="B57" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+    <row r="58" spans="1:30">
+      <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B51" s="4" t="s">
+    <row r="59" spans="1:30">
+      <c r="B59" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A52" s="8"/>
-      <c r="B52" s="9" t="s">
+    <row r="60" spans="1:30">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8"/>
-      <c r="O52" s="8"/>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="T52" s="8"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="8"/>
-      <c r="W52" s="8"/>
-      <c r="X52" s="8"/>
-      <c r="Y52" s="8"/>
-      <c r="Z52" s="8"/>
-      <c r="AA52" s="8"/>
-      <c r="AB52" s="8"/>
-      <c r="AC52" s="8"/>
-      <c r="AD52" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="8"/>
+      <c r="T60" s="8"/>
+      <c r="U60" s="8"/>
+      <c r="V60" s="8"/>
+      <c r="W60" s="8"/>
+      <c r="X60" s="8"/>
+      <c r="Y60" s="8"/>
+      <c r="Z60" s="8"/>
+      <c r="AA60" s="8"/>
+      <c r="AB60" s="8"/>
+      <c r="AC60" s="8"/>
+      <c r="AD60" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2384,354 +2521,354 @@
       <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>123</v>
       </c>
@@ -2748,14 +2885,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2774,164 +2911,164 @@
       <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="17.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1">
       <c r="A56" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" s="3" customFormat="1">
       <c r="A62" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
         <v>44</v>
       </c>
@@ -2952,94 +3089,94 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>25</v>
       </c>

</xml_diff>